<commit_message>
Update feature otentikasi menambahkan tag dan runner
</commit_message>
<xml_diff>
--- a/Digital Bootcamp Trainer/DataSet/trainer.xlsx
+++ b/Digital Bootcamp Trainer/DataSet/trainer.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Digital Bootcamp 79\Digital-Bootcamp\Digital Bootcamp Trainer\DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ABA27B-3EF0-4361-8A20-E0C9AEF682A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DA9391-47C2-4E0F-AA9B-AC14D11E3ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DB4E7776-A01A-435C-9307-61C4FEB4F0A7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Otentikasi" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>akhimusyafak@gmail.com</t>
   </si>
@@ -43,13 +43,55 @@
   </si>
   <si>
     <t>akhmad20221</t>
+  </si>
+  <si>
+    <t>akhimusyafak</t>
+  </si>
+  <si>
+    <t>akhmad20222</t>
+  </si>
+  <si>
+    <t>akhmad</t>
+  </si>
+  <si>
+    <t>akhmadmusyafak@gmail.com</t>
+  </si>
+  <si>
+    <t>TC-Login-001</t>
+  </si>
+  <si>
+    <t>TC-Login-002</t>
+  </si>
+  <si>
+    <t>TC-Login-003</t>
+  </si>
+  <si>
+    <t>TC-Login-004</t>
+  </si>
+  <si>
+    <t>TC-Login-005</t>
+  </si>
+  <si>
+    <t>TC-Login-006</t>
+  </si>
+  <si>
+    <t>TC-Login-007</t>
+  </si>
+  <si>
+    <t>TC-Login-008</t>
+  </si>
+  <si>
+    <t>TC-Login-009</t>
+  </si>
+  <si>
+    <t>TC-Login-010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +111,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -414,19 +462,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B699ADA1-552B-4253-9122-1049502024E6}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -434,19 +483,110 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{E5FAD35E-8993-431D-8850-A7F5C46F10BB}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{3CE7C16F-4B7C-4D51-8DD3-C7B1B62B9246}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{88F6EA73-53EA-405E-BAF0-A4F646BE53DB}"/>
+    <hyperlink ref="A7" r:id="rId3" xr:uid="{96B52F9F-253D-48F5-867B-BC8F8F48CC4E}"/>
+    <hyperlink ref="A10" r:id="rId4" xr:uid="{609ADB46-A0B0-4BBA-8E4D-8CB96E92C5FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Case Fitur Topik - Membuat Materi
</commit_message>
<xml_diff>
--- a/Digital Bootcamp Trainer/DataSet/trainer.xlsx
+++ b/Digital Bootcamp Trainer/DataSet/trainer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Digital Bootcamp 79\Digital-Bootcamp\Digital Bootcamp Trainer\DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01988D96-D1BC-4CE8-9F8E-736B10DE8DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE30ED3D-EF5D-482C-924D-672C9D47F42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{DB4E7776-A01A-435C-9307-61C4FEB4F0A7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
   <si>
     <t>akhimusyafak@gmail.com</t>
   </si>
@@ -125,6 +125,48 @@
   </si>
   <si>
     <t>java-logo.jpg</t>
+  </si>
+  <si>
+    <t>JAVA,FUNDAMENTAL,INPUT</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-001</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-002</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-003</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-004</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-005</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-006</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-007</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-008</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-009</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-010</t>
+  </si>
+  <si>
+    <t>TC-Membuat materi-011</t>
+  </si>
+  <si>
+    <t>ukuran lebih dari 2 MB</t>
+  </si>
+  <si>
+    <t>file extensi salah</t>
   </si>
 </sst>
 </file>
@@ -633,23 +675,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01538D8B-695A-4424-BF9E-1439C0D88565}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -672,7 +716,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -694,13 +738,215 @@
       <c r="G2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update terbaru fitur Daftar Bab
</commit_message>
<xml_diff>
--- a/Digital Bootcamp Trainer/DataSet/trainer.xlsx
+++ b/Digital Bootcamp Trainer/DataSet/trainer.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Digital Bootcamp 79\Digital-Bootcamp\Digital Bootcamp Trainer\DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE30ED3D-EF5D-482C-924D-672C9D47F42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F85BBF-E4D2-48B6-9A3B-ACB3F58DF0F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{DB4E7776-A01A-435C-9307-61C4FEB4F0A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Otentikasi" sheetId="1" r:id="rId1"/>
-    <sheet name="Topik" sheetId="2" r:id="rId2"/>
+    <sheet name="Daftar Topik" sheetId="2" r:id="rId2"/>
+    <sheet name="Daftar Bab" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="127">
   <si>
     <t>akhimusyafak@gmail.com</t>
   </si>
@@ -167,6 +168,252 @@
   </si>
   <si>
     <t>file extensi salah</t>
+  </si>
+  <si>
+    <t>Fundamental Selenium</t>
+  </si>
+  <si>
+    <t>Fundamental Selenium yang mengenalkan automation testing dari dasar.</t>
+  </si>
+  <si>
+    <t>FUNDAMENTAL</t>
+  </si>
+  <si>
+    <t>Sulit</t>
+  </si>
+  <si>
+    <t>Sembunyi</t>
+  </si>
+  <si>
+    <t>TC-Mengubah materi-001</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TC-Mengubah materi-002</t>
+  </si>
+  <si>
+    <t>TC-Mengubah materi-003</t>
+  </si>
+  <si>
+    <t>TC-Mengubah materi-004</t>
+  </si>
+  <si>
+    <t>TC-Mengubah materi-005</t>
+  </si>
+  <si>
+    <t>TC-Mengubah materi-006</t>
+  </si>
+  <si>
+    <t>TC-Mengubah materi-007</t>
+  </si>
+  <si>
+    <t>TC-Mengubah materi-008</t>
+  </si>
+  <si>
+    <t>TC-Menghapus materi-001</t>
+  </si>
+  <si>
+    <t>TC-Menghapus materi-002</t>
+  </si>
+  <si>
+    <t>TC-Menghapus materi-003</t>
+  </si>
+  <si>
+    <t>TC-Mengubah visibilitas materi-001</t>
+  </si>
+  <si>
+    <t>Pencarian</t>
+  </si>
+  <si>
+    <t>Fundamental</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-001</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Jawa</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-002</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-003</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-004</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-005</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-006</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-007</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-008</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-009</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-010</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-011</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-012</t>
+  </si>
+  <si>
+    <t>TC-Mencari materi-013</t>
+  </si>
+  <si>
+    <t>Bab</t>
+  </si>
+  <si>
+    <t>Topik</t>
+  </si>
+  <si>
+    <t>Skala</t>
+  </si>
+  <si>
+    <t>Pendahuluan Bahasa Java</t>
+  </si>
+  <si>
+    <t>Fundamental Java</t>
+  </si>
+  <si>
+    <t>Pendahuluan bahasa Java Fundamental Java</t>
+  </si>
+  <si>
+    <t>TC-Membuat Bab-001</t>
+  </si>
+  <si>
+    <t>TC-Membuat Bab-002</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>TC-Membuat Bab-003</t>
+  </si>
+  <si>
+    <t>TC-Membuat Bab-004</t>
+  </si>
+  <si>
+    <t>TC-Membuat Bab-005</t>
+  </si>
+  <si>
+    <t>TC-Membuat Bab-006</t>
+  </si>
+  <si>
+    <t>TC-Membuat Bab-007</t>
+  </si>
+  <si>
+    <t>TC-Membuat Bab-008</t>
+  </si>
+  <si>
+    <t>alifagungp</t>
+  </si>
+  <si>
+    <t>alif2505</t>
+  </si>
+  <si>
+    <t>Pendahuluan Bahasa Java 2</t>
+  </si>
+  <si>
+    <t>Pendahuluan bahasa Java Fundamental Java 2</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Bab-001</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Bab-002</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Bab-003</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Bab-004</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Bab-005</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Bab-006</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Bab-007</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Visibilitas-001</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>TC-Menghapus Bab-001</t>
+  </si>
+  <si>
+    <t>TC-Menghapus Bab-002</t>
+  </si>
+  <si>
+    <t>TC-Menghapus Bab-003</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-001</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-002</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-003</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-004</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-005</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-006</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-007</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-008</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-009</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-010</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-011</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-012</t>
+  </si>
+  <si>
+    <t>TC-Mencari Bab-013</t>
   </si>
 </sst>
 </file>
@@ -225,10 +472,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -544,16 +792,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B699ADA1-552B-4253-9122-1049502024E6}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -567,9 +817,15 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="H2" t="s">
@@ -577,10 +833,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="H3" t="s">
@@ -589,9 +851,15 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="H4" t="s">
@@ -599,10 +867,16 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="H5" t="s">
@@ -611,9 +885,15 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="H6" t="s">
@@ -621,10 +901,16 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>3</v>
       </c>
       <c r="H7" t="s">
@@ -632,7 +918,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
       <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
         <v>3</v>
       </c>
       <c r="H8" t="s">
@@ -641,6 +933,12 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="H9" t="s">
@@ -648,7 +946,13 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="s">
@@ -656,17 +960,259 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
       <c r="H11" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{3CE7C16F-4B7C-4D51-8DD3-C7B1B62B9246}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{88F6EA73-53EA-405E-BAF0-A4F646BE53DB}"/>
-    <hyperlink ref="A7" r:id="rId3" xr:uid="{96B52F9F-253D-48F5-867B-BC8F8F48CC4E}"/>
-    <hyperlink ref="A10" r:id="rId4" xr:uid="{609ADB46-A0B0-4BBA-8E4D-8CB96E92C5FE}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{A9ACAFE4-BDC0-4F35-AD8D-3D7919C1FB36}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{EB944611-821F-4270-8E1A-CC01B93BD1FB}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{627E3F4E-52EA-4ABD-BDC4-705A787D33B5}"/>
+    <hyperlink ref="C10" r:id="rId4" xr:uid="{832ED643-FCAE-4A67-99D8-4C170AD439E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -675,274 +1221,1047 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01538D8B-695A-4424-BF9E-1439C0D88565}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6328125" customWidth="1"/>
+    <col min="11" max="11" width="30.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="s">
+        <v>49</v>
+      </c>
+      <c r="J20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="H24" t="s">
+        <v>64</v>
+      </c>
+      <c r="J24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
+        <v>67</v>
+      </c>
+      <c r="J28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>48</v>
+      </c>
+      <c r="J31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
+        <v>66</v>
+      </c>
+      <c r="J32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>66</v>
+      </c>
+      <c r="J34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H36" t="s">
+        <v>49</v>
+      </c>
+      <c r="J36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E3A23F4-608E-4AD8-8510-06950C58DE67}">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
+      <c r="H1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
-        <v>26</v>
+      <c r="F2" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="G2" t="s">
         <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="K2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
-        <v>26</v>
+      <c r="F3" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="J3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
       <c r="J4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
-        <v>26</v>
+      <c r="F6" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>28</v>
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
+        <v>85</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="G7" t="s">
         <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
+      <c r="F8" s="3"/>
       <c r="G8" t="s">
         <v>27</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
+      <c r="F10" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="J10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
-      <c r="F12" t="s">
-        <v>26</v>
+      <c r="F12" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>110</v>
+      </c>
+      <c r="J20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
         <v>27</v>
       </c>
-      <c r="J12" t="s">
-        <v>42</v>
+      <c r="J22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>67</v>
+      </c>
+      <c r="J24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>110</v>
+      </c>
+      <c r="J25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>49</v>
+      </c>
+      <c r="J29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>66</v>
+      </c>
+      <c r="J30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
+        <v>49</v>
+      </c>
+      <c r="J32" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update fitur materi(Ubah, Hapus, Cari Video Pembahasan)
</commit_message>
<xml_diff>
--- a/Digital Bootcamp Trainer/DataSet/trainer.xlsx
+++ b/Digital Bootcamp Trainer/DataSet/trainer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Digital Bootcamp 79\Digital-Bootcamp\Digital Bootcamp Trainer\DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE8F81C-889F-4E4B-9BF6-409CC5FEDF3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B98FC6E-8FCC-41E3-8DE1-F6360FE4BFEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB4E7776-A01A-435C-9307-61C4FEB4F0A7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="240">
   <si>
     <t>akhimusyafak@gmail.com</t>
   </si>
@@ -593,6 +593,168 @@
   </si>
   <si>
     <t>padepokan79oke.com</t>
+  </si>
+  <si>
+    <t>ukuran tidak sesuai</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-001</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-002</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-003</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-004</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-005</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-006</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-007</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-008</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-009</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-010</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-011</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-012</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-013</t>
+  </si>
+  <si>
+    <t>TC-Membuat Video Pembahasan-014</t>
+  </si>
+  <si>
+    <t>Materi pembahasan Selenium</t>
+  </si>
+  <si>
+    <t>padepokan79oke2.com</t>
+  </si>
+  <si>
+    <t>Fundamental Selenium yang mengenalkan java dari dasar.</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Video Pembahasan-001</t>
+  </si>
+  <si>
+    <t>tidak sesuai</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Video Pembahasan-002</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Video Pembahasan-003</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Video Pembahasan-004</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Video Pembahasan-005</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Video Pembahasan-006</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Video Pembahasan-007</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Video Pembahasan-008</t>
+  </si>
+  <si>
+    <t>TC-Mengubah Video Pembahasan-009</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Pembahasan</t>
+  </si>
+  <si>
+    <t>Pendahuluan</t>
+  </si>
+  <si>
+    <t>Foreeach</t>
+  </si>
+  <si>
+    <t>TC-Menghapus Video Pembahasan-001</t>
+  </si>
+  <si>
+    <t>TC-Menghapus Video Pembahasan-002</t>
+  </si>
+  <si>
+    <t>TC-Menghapus Video Pembahasan-003</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-001</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-002</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-003</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-004</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-005</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-006</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-007</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-008</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-009</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-010</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-011</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-012</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-013</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-014</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-015</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-016</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-017</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-018</t>
+  </si>
+  <si>
+    <t>TC-Mencari Video Pembahasan-019</t>
   </si>
 </sst>
 </file>
@@ -975,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B699ADA1-552B-4253-9122-1049502024E6}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91:B100"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2969,7 +3131,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3520,22 +3682,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5AF6A6-D50D-4037-84FD-E39AF107C9E0}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="F36" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -3611,6 +3774,9 @@
       <c r="L2" s="3" t="s">
         <v>183</v>
       </c>
+      <c r="N2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -3643,8 +3809,841 @@
       <c r="L3" s="3" t="s">
         <v>183</v>
       </c>
+      <c r="N3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I4" t="s">
+        <v>184</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I5" t="s">
+        <v>184</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" t="s">
+        <v>158</v>
+      </c>
+      <c r="I6" t="s">
+        <v>184</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I7" t="s">
+        <v>184</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I8" t="s">
+        <v>184</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" t="s">
+        <v>158</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" t="s">
+        <v>158</v>
+      </c>
+      <c r="I12" t="s">
+        <v>184</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" t="s">
+        <v>158</v>
+      </c>
+      <c r="I13" t="s">
+        <v>184</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="N13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" t="s">
+        <v>158</v>
+      </c>
+      <c r="I15" t="s">
+        <v>184</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" t="s">
+        <v>203</v>
+      </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" t="s">
+        <v>158</v>
+      </c>
+      <c r="I16" t="s">
+        <v>184</v>
+      </c>
+      <c r="J16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" t="s">
+        <v>47</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" t="s">
+        <v>158</v>
+      </c>
+      <c r="I18" t="s">
+        <v>184</v>
+      </c>
+      <c r="J18" t="s">
+        <v>49</v>
+      </c>
+      <c r="K18" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N18" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C19" t="s">
+        <v>205</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" t="s">
+        <v>158</v>
+      </c>
+      <c r="I19" t="s">
+        <v>184</v>
+      </c>
+      <c r="J19" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>203</v>
+      </c>
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" t="s">
+        <v>158</v>
+      </c>
+      <c r="I20" t="s">
+        <v>184</v>
+      </c>
+      <c r="J20" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" t="s">
+        <v>47</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B21" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" t="s">
+        <v>158</v>
+      </c>
+      <c r="I21" t="s">
+        <v>184</v>
+      </c>
+      <c r="J21" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" t="s">
+        <v>47</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N21" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E22" t="s">
+        <v>203</v>
+      </c>
+      <c r="F22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" t="s">
+        <v>158</v>
+      </c>
+      <c r="I22" t="s">
+        <v>184</v>
+      </c>
+      <c r="J22" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="N22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23" t="s">
+        <v>203</v>
+      </c>
+      <c r="F23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" t="s">
+        <v>184</v>
+      </c>
+      <c r="J23" t="s">
+        <v>49</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E24" t="s">
+        <v>203</v>
+      </c>
+      <c r="F24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" t="s">
+        <v>158</v>
+      </c>
+      <c r="I24" t="s">
+        <v>184</v>
+      </c>
+      <c r="J24" t="s">
+        <v>49</v>
+      </c>
+      <c r="K24" t="s">
+        <v>47</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N24" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N25" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N26" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N27" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
+        <v>215</v>
+      </c>
+      <c r="N28" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>216</v>
+      </c>
+      <c r="N29" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>66</v>
+      </c>
+      <c r="N30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>217</v>
+      </c>
+      <c r="N31" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+      <c r="N32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>49</v>
+      </c>
+      <c r="N33" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>67</v>
+      </c>
+      <c r="N34" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>215</v>
+      </c>
+      <c r="N35" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="36" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H36" t="s">
+        <v>49</v>
+      </c>
+      <c r="N36" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H37" t="s">
+        <v>217</v>
+      </c>
+      <c r="N37" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>49</v>
+      </c>
+      <c r="N38" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="39" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H39" t="s">
+        <v>66</v>
+      </c>
+      <c r="N39" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="40" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H40" t="s">
+        <v>49</v>
+      </c>
+      <c r="N40" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H41" t="s">
+        <v>216</v>
+      </c>
+      <c r="N41" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H42" t="s">
+        <v>49</v>
+      </c>
+      <c r="N42" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="43" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H43" t="s">
+        <v>25</v>
+      </c>
+      <c r="N43" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="44" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H44" t="s">
+        <v>49</v>
+      </c>
+      <c r="N44" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H45" t="s">
+        <v>49</v>
+      </c>
+      <c r="N45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="46" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H46" t="s">
+        <v>66</v>
+      </c>
+      <c r="N46" t="s">
+        <v>239</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>